<commit_message>
validity of sudoku with back-tracking - tested on 1M boards/solutions
</commit_message>
<xml_diff>
--- a/MILP - Approach/grid/grid-7-2.xlsx
+++ b/MILP - Approach/grid/grid-7-2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/83726ec0a80c1546/Python/Experiments/Pyomo/_Solver Max/Crossword/grid/Github/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parzi\OneDrive - Tribhuvan University\Desktop\Major Project\CODE\BCS Code\BCS-ALL-Code\Crossword Generator\MILP - Approach\grid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="8_{A9BCF097-E2D3-4E52-ACF6-72A17EC75F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CF8221D-F33E-4AAC-9E43-AF7F55C6D935}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901AF39F-8456-4C5A-8E09-512854E40594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{324EC751-9C60-40DD-8432-DBCA825DD949}"/>
+    <workbookView xWindow="-23148" yWindow="-1044" windowWidth="23256" windowHeight="12456" xr2:uid="{324EC751-9C60-40DD-8432-DBCA825DD949}"/>
   </bookViews>
   <sheets>
     <sheet name="Grid" sheetId="1" r:id="rId1"/>
@@ -57,27 +57,19 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -452,9 +444,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -492,7 +484,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -598,7 +590,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -740,7 +732,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -751,7 +743,7 @@
   <dimension ref="B1:S19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>